<commit_message>
add predictions 2022-2023 Prophet
</commit_message>
<xml_diff>
--- a/notebooks/Prophet/predictions_opzh.xlsx
+++ b/notebooks/Prophet/predictions_opzh.xlsx
@@ -462,11 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C2" t="n">
+        <v>73.03</v>
+      </c>
       <c r="D2" t="n">
-        <v>64.84607701767798</v>
+        <v>68.93029213826965</v>
       </c>
     </row>
     <row r="3">
@@ -476,11 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C3" t="n">
+        <v>73.7</v>
+      </c>
       <c r="D3" t="n">
-        <v>63.1460761207472</v>
+        <v>67.16399675151141</v>
       </c>
     </row>
     <row r="4">
@@ -490,11 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C4" t="n">
+        <v>71.22</v>
+      </c>
       <c r="D4" t="n">
-        <v>65.54582179656995</v>
+        <v>66.79542453433307</v>
       </c>
     </row>
     <row r="5">
@@ -504,11 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>71.98</v>
+      </c>
       <c r="D5" t="n">
-        <v>63.60582131168322</v>
+        <v>65.00247694046756</v>
       </c>
     </row>
     <row r="6">
@@ -518,11 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C6" t="n">
+        <v>70.8</v>
+      </c>
       <c r="D6" t="n">
-        <v>61.72875420057601</v>
+        <v>66.47871967484677</v>
       </c>
     </row>
     <row r="7">
@@ -532,11 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C7" t="n">
+        <v>71.62</v>
+      </c>
       <c r="D7" t="n">
-        <v>59.84875424815697</v>
+        <v>64.63648555243927</v>
       </c>
     </row>
     <row r="8">
@@ -546,11 +558,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C8" t="n">
+        <v>72.45</v>
+      </c>
       <c r="D8" t="n">
-        <v>64.10759897619761</v>
+        <v>67.75903239815268</v>
       </c>
     </row>
     <row r="9">
@@ -560,11 +574,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C9" t="n">
+        <v>72.91</v>
+      </c>
       <c r="D9" t="n">
-        <v>61.74759894341514</v>
+        <v>65.79576115103079</v>
       </c>
     </row>
     <row r="10">
@@ -574,11 +590,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C10" t="n">
+        <v>70.56999999999999</v>
+      </c>
       <c r="D10" t="n">
-        <v>63.18873359060169</v>
+        <v>67.15554954918417</v>
       </c>
     </row>
     <row r="11">
@@ -588,11 +606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>71.18000000000001</v>
+      </c>
       <c r="D11" t="n">
-        <v>61.51873373334216</v>
+        <v>65.72098489234084</v>
       </c>
     </row>
     <row r="12">
@@ -602,11 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C12" t="n">
+        <v>72.48</v>
+      </c>
       <c r="D12" t="n">
-        <v>65.30065372117602</v>
+        <v>68.21253443853563</v>
       </c>
     </row>
     <row r="13">
@@ -616,11 +638,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>73.08</v>
+      </c>
       <c r="D13" t="n">
-        <v>64.16065341611832</v>
+        <v>66.74608152266929</v>
       </c>
     </row>
     <row r="14">
@@ -630,11 +654,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C14" t="n">
+        <v>69.90000000000001</v>
+      </c>
       <c r="D14" t="n">
-        <v>62.72945157814578</v>
+        <v>66.37467423029474</v>
       </c>
     </row>
     <row r="15">
@@ -644,11 +670,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C15" t="n">
+        <v>71.05</v>
+      </c>
       <c r="D15" t="n">
-        <v>60.47945235983943</v>
+        <v>64.54131458103379</v>
       </c>
     </row>
     <row r="16">
@@ -658,11 +686,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C16" t="n">
+        <v>71.54000000000001</v>
+      </c>
       <c r="D16" t="n">
-        <v>62.82308599604229</v>
+        <v>66.71564807401873</v>
       </c>
     </row>
     <row r="17">
@@ -672,11 +702,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C17" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C17" t="n">
+        <v>72.45</v>
+      </c>
       <c r="D17" t="n">
-        <v>60.88308568364465</v>
+        <v>64.88572551726357</v>
       </c>
     </row>
     <row r="18">
@@ -686,11 +718,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C18" t="n">
+        <v>72.12</v>
+      </c>
       <c r="D18" t="n">
-        <v>60.48687106296385</v>
+        <v>66.34183994641711</v>
       </c>
     </row>
     <row r="19">
@@ -700,11 +734,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C19" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C19" t="n">
+        <v>72.44</v>
+      </c>
       <c r="D19" t="n">
-        <v>58.52687138119837</v>
+        <v>64.06165282182003</v>
       </c>
     </row>
     <row r="20">
@@ -714,11 +750,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C20" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C20" t="n">
+        <v>73.78</v>
+      </c>
       <c r="D20" t="n">
-        <v>65.23553097829952</v>
+        <v>69.60509046993057</v>
       </c>
     </row>
     <row r="21">
@@ -728,11 +766,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C21" t="n">
+        <v>74.48999999999999</v>
+      </c>
       <c r="D21" t="n">
-        <v>64.00552968833253</v>
+        <v>67.97245982573301</v>
       </c>
     </row>
     <row r="22">
@@ -742,11 +782,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C22" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C22" t="n">
+        <v>70.73</v>
+      </c>
       <c r="D22" t="n">
-        <v>62.42355179291334</v>
+        <v>67.08515388982207</v>
       </c>
     </row>
     <row r="23">
@@ -756,11 +798,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C23" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C23" t="n">
+        <v>71.65000000000001</v>
+      </c>
       <c r="D23" t="n">
-        <v>61.30355148029497</v>
+        <v>65.41791077303469</v>
       </c>
     </row>
     <row r="24">
@@ -770,11 +814,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C24" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C24" t="n">
+        <v>72.14</v>
+      </c>
       <c r="D24" t="n">
-        <v>62.95920551758219</v>
+        <v>66.57227053669482</v>
       </c>
     </row>
     <row r="25">
@@ -784,11 +830,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C25" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C25" t="n">
+        <v>73.19</v>
+      </c>
       <c r="D25" t="n">
-        <v>60.70920626628369</v>
+        <v>64.35546897504513</v>
       </c>
     </row>
     <row r="26">
@@ -798,11 +846,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C26" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C26" t="n">
+        <v>70.34999999999999</v>
+      </c>
       <c r="D26" t="n">
-        <v>61.1369658299861</v>
+        <v>65.81040814241285</v>
       </c>
     </row>
     <row r="27">
@@ -812,11 +862,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C27" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C27" t="n">
+        <v>71.47</v>
+      </c>
       <c r="D27" t="n">
-        <v>59.01696587752438</v>
+        <v>63.84865538052858</v>
       </c>
     </row>
     <row r="28">
@@ -826,11 +878,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C28" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C28" t="n">
+        <v>72.01000000000001</v>
+      </c>
       <c r="D28" t="n">
-        <v>62.68958851795412</v>
+        <v>68.16351976642223</v>
       </c>
     </row>
     <row r="29">
@@ -840,11 +894,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C29" t="n">
+        <v>72.87</v>
+      </c>
       <c r="D29" t="n">
-        <v>60.8495887717612</v>
+        <v>66.40217077737471</v>
       </c>
     </row>
     <row r="30">
@@ -854,11 +910,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C30" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C30" t="n">
+        <v>69.94</v>
+      </c>
       <c r="D30" t="n">
-        <v>63.19865442345734</v>
+        <v>66.30484946799656</v>
       </c>
     </row>
     <row r="31">
@@ -868,11 +926,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C31" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C31" t="n">
+        <v>70.61</v>
+      </c>
       <c r="D31" t="n">
-        <v>61.33865432540871</v>
+        <v>64.6578559534248</v>
       </c>
     </row>
     <row r="32">
@@ -882,11 +942,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C32" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C32" t="n">
+        <v>71.86</v>
+      </c>
       <c r="D32" t="n">
-        <v>64.86669922723398</v>
+        <v>67.91959057107192</v>
       </c>
     </row>
     <row r="33">
@@ -896,11 +958,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C33" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C33" t="n">
+        <v>72.15000000000001</v>
+      </c>
       <c r="D33" t="n">
-        <v>63.72669862332244</v>
+        <v>66.41412849058419</v>
       </c>
     </row>
     <row r="34">
@@ -910,11 +974,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C34" t="n">
+        <v>71.55</v>
+      </c>
       <c r="D34" t="n">
-        <v>62.59487011914325</v>
+        <v>66.84621386249816</v>
       </c>
     </row>
     <row r="35">
@@ -924,11 +990,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C35" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C35" t="n">
+        <v>71.98999999999999</v>
+      </c>
       <c r="D35" t="n">
-        <v>60.68487003098568</v>
+        <v>64.88959067202408</v>
       </c>
     </row>
     <row r="36">
@@ -938,11 +1006,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C36" t="n">
+        <v>78.17</v>
+      </c>
       <c r="D36" t="n">
-        <v>68.14755153180532</v>
+        <v>72.80443020182025</v>
       </c>
     </row>
     <row r="37">
@@ -952,11 +1022,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C37" t="n">
+        <v>79.38</v>
+      </c>
       <c r="D37" t="n">
-        <v>66.64755231953573</v>
+        <v>71.08145542160594</v>
       </c>
     </row>
     <row r="38">
@@ -966,11 +1038,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C38" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C38" t="n">
+        <v>69.03</v>
+      </c>
       <c r="D38" t="n">
-        <v>57.94701120615737</v>
+        <v>64.00064968520363</v>
       </c>
     </row>
     <row r="39">
@@ -980,11 +1054,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C39" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C39" t="n">
+        <v>69.75</v>
+      </c>
       <c r="D39" t="n">
-        <v>55.53701144379474</v>
+        <v>61.83779309067379</v>
       </c>
     </row>
     <row r="40">
@@ -994,11 +1070,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C40" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C40" t="n">
+        <v>69.94</v>
+      </c>
       <c r="D40" t="n">
-        <v>61.77418753230107</v>
+        <v>66.21282119049799</v>
       </c>
     </row>
     <row r="41">
@@ -1008,11 +1086,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C41" t="n">
+        <v>70.43000000000001</v>
+      </c>
       <c r="D41" t="n">
-        <v>59.62418746308609</v>
+        <v>64.65625204310165</v>
       </c>
     </row>
     <row r="42">
@@ -1022,11 +1102,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C42" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C42" t="n">
+        <v>70.93000000000001</v>
+      </c>
       <c r="D42" t="n">
-        <v>64.51302913932045</v>
+        <v>67.41266030993944</v>
       </c>
     </row>
     <row r="43">
@@ -1036,11 +1118,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C43" t="n">
+        <v>71.51000000000001</v>
+      </c>
       <c r="D43" t="n">
-        <v>62.69302925772371</v>
+        <v>66.0002782963103</v>
       </c>
     </row>
     <row r="44">
@@ -1050,11 +1134,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C44" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C44" t="n">
+        <v>70.73999999999999</v>
+      </c>
       <c r="D44" t="n">
-        <v>63.70398050349783</v>
+        <v>66.88852646787981</v>
       </c>
     </row>
     <row r="45">
@@ -1064,11 +1150,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C45" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C45" t="n">
+        <v>70.67</v>
+      </c>
       <c r="D45" t="n">
-        <v>62.41568360601923</v>
+        <v>65.23848611845921</v>
       </c>
     </row>
     <row r="46">
@@ -1078,11 +1166,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C46" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C46" t="n">
+        <v>71.56</v>
+      </c>
       <c r="D46" t="n">
-        <v>68.26101282340981</v>
+        <v>67.81982453379202</v>
       </c>
     </row>
     <row r="47">
@@ -1092,11 +1182,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C47" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C47" t="n">
+        <v>71.7</v>
+      </c>
       <c r="D47" t="n">
-        <v>66.64101268762148</v>
+        <v>66.48222498134204</v>
       </c>
     </row>
     <row r="48">
@@ -1106,11 +1198,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C48" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C48" t="n">
+        <v>73.06999999999999</v>
+      </c>
       <c r="D48" t="n">
-        <v>66.31724593277161</v>
+        <v>70.11514161138805</v>
       </c>
     </row>
     <row r="49">
@@ -1120,11 +1214,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C49" t="n">
+        <v>73.70999999999999</v>
+      </c>
       <c r="D49" t="n">
-        <v>64.39724583197768</v>
+        <v>68.94898912328496</v>
       </c>
     </row>
     <row r="50">
@@ -1134,11 +1230,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C50" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C50" t="n">
+        <v>73.33</v>
+      </c>
       <c r="D50" t="n">
-        <v>66.18718626356686</v>
+        <v>69.00494205866215</v>
       </c>
     </row>
     <row r="51">
@@ -1148,11 +1246,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C51" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C51" t="n">
+        <v>74.88</v>
+      </c>
       <c r="D51" t="n">
-        <v>64.95718673603702</v>
+        <v>67.42052711889343</v>
       </c>
     </row>
     <row r="52">
@@ -1162,11 +1262,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C52" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C52" t="n">
+        <v>70.16</v>
+      </c>
       <c r="D52" t="n">
-        <v>60.86941253589402</v>
+        <v>65.46547810748615</v>
       </c>
     </row>
     <row r="53">
@@ -1176,11 +1278,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C53" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C53" t="n">
+        <v>70.44</v>
+      </c>
       <c r="D53" t="n">
-        <v>59.27941281419801</v>
+        <v>63.63821851675389</v>
       </c>
     </row>
     <row r="54">
@@ -1190,11 +1294,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C54" t="n">
+        <v>70.45</v>
+      </c>
       <c r="D54" t="n">
-        <v>64.29643872980704</v>
+        <v>66.26780110122331</v>
       </c>
     </row>
     <row r="55">
@@ -1204,11 +1310,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C55" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C55" t="n">
+        <v>70.43000000000001</v>
+      </c>
       <c r="D55" t="n">
-        <v>62.36643839358963</v>
+        <v>64.86616598510173</v>
       </c>
     </row>
     <row r="56">
@@ -1218,11 +1326,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C56" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C56" t="n">
+        <v>68.95</v>
+      </c>
       <c r="D56" t="n">
-        <v>62.29157992657248</v>
+        <v>65.95577046856178</v>
       </c>
     </row>
     <row r="57">
@@ -1232,11 +1342,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C57" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C57" t="n">
+        <v>70</v>
+      </c>
       <c r="D57" t="n">
-        <v>60.87157952852066</v>
+        <v>64.48847919297536</v>
       </c>
     </row>
     <row r="58">
@@ -1246,11 +1358,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C58" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C58" t="n">
+        <v>75.77</v>
+      </c>
       <c r="D58" t="n">
-        <v>66.47501701164094</v>
+        <v>71.03822870968892</v>
       </c>
     </row>
     <row r="59">
@@ -1260,11 +1374,13 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C59" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C59" t="n">
+        <v>76.55</v>
+      </c>
       <c r="D59" t="n">
-        <v>65.13501457513529</v>
+        <v>69.30892217448383</v>
       </c>
     </row>
     <row r="60">
@@ -1274,11 +1390,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C60" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C60" t="n">
+        <v>73.59999999999999</v>
+      </c>
       <c r="D60" t="n">
-        <v>70.12450607578923</v>
+        <v>70.83647447748849</v>
       </c>
     </row>
     <row r="61">
@@ -1288,11 +1406,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C61" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C61" t="n">
+        <v>75.36</v>
+      </c>
       <c r="D61" t="n">
-        <v>68.20450628350538</v>
+        <v>69.6877354606777</v>
       </c>
     </row>
     <row r="62">
@@ -1302,11 +1422,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C62" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C62" t="n">
+        <v>73.48999999999999</v>
+      </c>
       <c r="D62" t="n">
-        <v>66.37858988227092</v>
+        <v>69.41043245450226</v>
       </c>
     </row>
     <row r="63">
@@ -1316,11 +1438,13 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C63" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C63" t="n">
+        <v>74.53</v>
+      </c>
       <c r="D63" t="n">
-        <v>64.85858878321301</v>
+        <v>67.72557904526558</v>
       </c>
     </row>
     <row r="64">
@@ -1330,11 +1454,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C64" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C64" t="n">
+        <v>71.97</v>
+      </c>
       <c r="D64" t="n">
-        <v>64.35618043558925</v>
+        <v>68.25150347827052</v>
       </c>
     </row>
     <row r="65">
@@ -1344,11 +1470,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C65" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C65" t="n">
+        <v>72.76000000000001</v>
+      </c>
       <c r="D65" t="n">
-        <v>62.8761810020297</v>
+        <v>66.75863634507431</v>
       </c>
     </row>
     <row r="66">
@@ -1358,11 +1486,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C66" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C66" t="n">
+        <v>72.92</v>
+      </c>
       <c r="D66" t="n">
-        <v>67.7328904437867</v>
+        <v>69.14158872285333</v>
       </c>
     </row>
     <row r="67">
@@ -1372,11 +1502,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C67" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C67" t="n">
+        <v>73.70999999999999</v>
+      </c>
       <c r="D67" t="n">
-        <v>66.06289070619786</v>
+        <v>67.50387885335313</v>
       </c>
     </row>
     <row r="68">
@@ -1386,11 +1518,13 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C68" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C68" t="n">
+        <v>71.8</v>
+      </c>
       <c r="D68" t="n">
-        <v>62.98850680076424</v>
+        <v>67.27562499646929</v>
       </c>
     </row>
     <row r="69">
@@ -1400,11 +1534,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C69" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C69" t="n">
+        <v>72.2</v>
+      </c>
       <c r="D69" t="n">
-        <v>60.97850666798858</v>
+        <v>65.37574206115553</v>
       </c>
     </row>
     <row r="70">
@@ -1414,11 +1550,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C70" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C70" t="n">
+        <v>73.23999999999999</v>
+      </c>
       <c r="D70" t="n">
-        <v>62.32509089902643</v>
+        <v>68.10224816603709</v>
       </c>
     </row>
     <row r="71">
@@ -1428,11 +1566,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C71" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C71" t="n">
+        <v>73.69</v>
+      </c>
       <c r="D71" t="n">
-        <v>60.35509019239264</v>
+        <v>66.1052522658055</v>
       </c>
     </row>
     <row r="72">
@@ -1442,11 +1582,13 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C72" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C72" t="n">
+        <v>72</v>
+      </c>
       <c r="D72" t="n">
-        <v>66.52000277906075</v>
+        <v>68.11118782937223</v>
       </c>
     </row>
     <row r="73">
@@ -1456,11 +1598,13 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C73" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C73" t="n">
+        <v>73.48</v>
+      </c>
       <c r="D73" t="n">
-        <v>64.34000272217703</v>
+        <v>66.24416946486561</v>
       </c>
     </row>
     <row r="74">
@@ -1470,11 +1614,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C74" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C74" t="n">
+        <v>74.56999999999999</v>
+      </c>
       <c r="D74" t="n">
-        <v>68.65348091938446</v>
+        <v>72.56631150738474</v>
       </c>
     </row>
     <row r="75">
@@ -1484,11 +1630,13 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C75" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C75" t="n">
+        <v>76.11</v>
+      </c>
       <c r="D75" t="n">
-        <v>66.94348139542075</v>
+        <v>71.89004199460582</v>
       </c>
     </row>
     <row r="76">
@@ -1498,11 +1646,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C76" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C76" t="n">
+        <v>78.22</v>
+      </c>
       <c r="D76" t="n">
-        <v>72.71516378627553</v>
+        <v>74.73888939437269</v>
       </c>
     </row>
     <row r="77">
@@ -1512,11 +1662,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C77" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C77" t="n">
+        <v>79.87</v>
+      </c>
       <c r="D77" t="n">
-        <v>72.59516373268964</v>
+        <v>73.49114007476642</v>
       </c>
     </row>
     <row r="78">
@@ -1526,11 +1678,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C78" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C78" t="n">
+        <v>78.34</v>
+      </c>
       <c r="D78" t="n">
-        <v>68.61201585190608</v>
+        <v>73.69807931835975</v>
       </c>
     </row>
     <row r="79">
@@ -1540,11 +1694,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C79" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C79" t="n">
+        <v>79.2</v>
+      </c>
       <c r="D79" t="n">
-        <v>67.23201533086285</v>
+        <v>71.78886273662886</v>
       </c>
     </row>
     <row r="80">
@@ -1554,11 +1710,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C80" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C80" t="n">
+        <v>75.51000000000001</v>
+      </c>
       <c r="D80" t="n">
-        <v>68.64635291029401</v>
+        <v>72.1145200904276</v>
       </c>
     </row>
     <row r="81">
@@ -1568,11 +1726,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C81" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C81" t="n">
+        <v>77.14</v>
+      </c>
       <c r="D81" t="n">
-        <v>68.03635662899879</v>
+        <v>70.8443054649896</v>
       </c>
     </row>
     <row r="82">
@@ -1582,11 +1742,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C82" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C82" t="n">
+        <v>75.31999999999999</v>
+      </c>
       <c r="D82" t="n">
-        <v>67.71065567437819</v>
+        <v>71.57460106155162</v>
       </c>
     </row>
     <row r="83">
@@ -1596,11 +1758,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C83" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C83" t="n">
+        <v>76.25</v>
+      </c>
       <c r="D83" t="n">
-        <v>66.34065560145564</v>
+        <v>70.20148888424325</v>
       </c>
     </row>
     <row r="84">
@@ -1610,11 +1774,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C84" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C84" t="n">
+        <v>74.7</v>
+      </c>
       <c r="D84" t="n">
-        <v>67.62680480654102</v>
+        <v>70.75475663090234</v>
       </c>
     </row>
     <row r="85">
@@ -1624,11 +1790,13 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C85" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C85" t="n">
+        <v>76.16</v>
+      </c>
       <c r="D85" t="n">
-        <v>66.08680506418143</v>
+        <v>69.21187727250529</v>
       </c>
     </row>
     <row r="86">
@@ -1638,11 +1806,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C86" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C86" t="n">
+        <v>74.61</v>
+      </c>
       <c r="D86" t="n">
-        <v>68.06435403686405</v>
+        <v>71.63903056006821</v>
       </c>
     </row>
     <row r="87">
@@ -1652,11 +1822,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C87" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C87" t="n">
+        <v>76.26000000000001</v>
+      </c>
       <c r="D87" t="n">
-        <v>68.15957126828752</v>
+        <v>70.78451210590842</v>
       </c>
     </row>
     <row r="88">
@@ -1666,11 +1838,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C88" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C88" t="n">
+        <v>74.29000000000001</v>
+      </c>
       <c r="D88" t="n">
-        <v>68.94628724042377</v>
+        <v>70.58510540418965</v>
       </c>
     </row>
     <row r="89">
@@ -1680,11 +1854,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C89" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C89" t="n">
+        <v>74.86</v>
+      </c>
       <c r="D89" t="n">
-        <v>67.50628783494341</v>
+        <v>69.18734375210774</v>
       </c>
     </row>
     <row r="90">
@@ -1694,11 +1870,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C90" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C90" t="n">
+        <v>72.98</v>
+      </c>
       <c r="D90" t="n">
-        <v>64.72359392727267</v>
+        <v>68.15281286313807</v>
       </c>
     </row>
     <row r="91">
@@ -1708,11 +1886,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C91" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C91" t="n">
+        <v>73.17</v>
+      </c>
       <c r="D91" t="n">
-        <v>63.90359444109355</v>
+        <v>66.69055459416484</v>
       </c>
     </row>
     <row r="92">
@@ -1722,11 +1902,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C92" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C92" t="n">
+        <v>71.90000000000001</v>
+      </c>
       <c r="D92" t="n">
-        <v>63.06358653459897</v>
+        <v>67.87736414038362</v>
       </c>
     </row>
     <row r="93">
@@ -1736,11 +1918,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C93" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C93" t="n">
+        <v>72.04000000000001</v>
+      </c>
       <c r="D93" t="n">
-        <v>61.50358641999511</v>
+        <v>66.20339405874127</v>
       </c>
     </row>
     <row r="94">
@@ -1750,11 +1934,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C94" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C94" t="n">
+        <v>73.16</v>
+      </c>
       <c r="D94" t="n">
-        <v>64.78174629041362</v>
+        <v>68.67946332307567</v>
       </c>
     </row>
     <row r="95">
@@ -1764,11 +1950,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C95" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C95" t="n">
+        <v>73.78</v>
+      </c>
       <c r="D95" t="n">
-        <v>63.47174608805202</v>
+        <v>66.92246367444096</v>
       </c>
     </row>
     <row r="96">
@@ -1778,11 +1966,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C96" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C96" t="n">
+        <v>74.92</v>
+      </c>
       <c r="D96" t="n">
-        <v>65.69079439940946</v>
+        <v>69.77942046174161</v>
       </c>
     </row>
     <row r="97">
@@ -1792,11 +1982,13 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C97" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C97" t="n">
+        <v>75.25</v>
+      </c>
       <c r="D97" t="n">
-        <v>64.43079450690261</v>
+        <v>68.04252105278367</v>
       </c>
     </row>
     <row r="98">
@@ -1806,11 +1998,13 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C98" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C98" t="n">
+        <v>72.13</v>
+      </c>
       <c r="D98" t="n">
-        <v>64.2683633620359</v>
+        <v>68.15287855516823</v>
       </c>
     </row>
     <row r="99">
@@ -1820,11 +2014,13 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C99" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C99" t="n">
+        <v>72.34</v>
+      </c>
       <c r="D99" t="n">
-        <v>63.17836336001193</v>
+        <v>66.73061828390904</v>
       </c>
     </row>
     <row r="100">
@@ -1834,11 +2030,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C100" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C100" t="n">
+        <v>72.48999999999999</v>
+      </c>
       <c r="D100" t="n">
-        <v>62.54251855730359</v>
+        <v>68.0315982677085</v>
       </c>
     </row>
     <row r="101">
@@ -1848,11 +2046,13 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C101" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C101" t="n">
+        <v>73.06999999999999</v>
+      </c>
       <c r="D101" t="n">
-        <v>61.4825186147641</v>
+        <v>66.35893150048379</v>
       </c>
     </row>
     <row r="102">
@@ -1862,11 +2062,13 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C102" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C102" t="n">
+        <v>70.90000000000001</v>
+      </c>
       <c r="D102" t="n">
-        <v>65.32526588254336</v>
+        <v>66.99870792725861</v>
       </c>
     </row>
     <row r="103">
@@ -1876,11 +2078,13 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C103" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C103" t="n">
+        <v>70.94</v>
+      </c>
       <c r="D103" t="n">
-        <v>64.25526587377681</v>
+        <v>65.63747956806644</v>
       </c>
     </row>
     <row r="104">
@@ -1890,11 +2094,13 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C104" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C104" t="n">
+        <v>71.31</v>
+      </c>
       <c r="D104" t="n">
-        <v>62.12289070522871</v>
+        <v>67.41439508966357</v>
       </c>
     </row>
     <row r="105">
@@ -1904,11 +2110,13 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C105" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C105" t="n">
+        <v>71.98999999999999</v>
+      </c>
       <c r="D105" t="n">
-        <v>60.33289154156955</v>
+        <v>65.71855952317664</v>
       </c>
     </row>
     <row r="106">
@@ -1918,11 +2126,13 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C106" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C106" t="n">
+        <v>71.48999999999999</v>
+      </c>
       <c r="D106" t="n">
-        <v>61.7601861823058</v>
+        <v>67.064882706945</v>
       </c>
     </row>
     <row r="107">
@@ -1932,11 +2142,13 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C107" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C107" t="n">
+        <v>72.09999999999999</v>
+      </c>
       <c r="D107" t="n">
-        <v>60.36018610211465</v>
+        <v>65.40283994045807</v>
       </c>
     </row>
     <row r="108">
@@ -1946,11 +2158,13 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C108" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C108" t="n">
+        <v>71.23999999999999</v>
+      </c>
       <c r="D108" t="n">
-        <v>63.5228671578089</v>
+        <v>65.93943175890745</v>
       </c>
     </row>
     <row r="109">
@@ -1960,11 +2174,13 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C109" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C109" t="n">
+        <v>71.12</v>
+      </c>
       <c r="D109" t="n">
-        <v>61.99286731197593</v>
+        <v>64.03590701393557</v>
       </c>
     </row>
     <row r="110">
@@ -1974,11 +2190,13 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C110" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C110" t="n">
+        <v>72.06999999999999</v>
+      </c>
       <c r="D110" t="n">
-        <v>62.44096679295503</v>
+        <v>67.90339563943279</v>
       </c>
     </row>
     <row r="111">
@@ -1988,11 +2206,13 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C111" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C111" t="n">
+        <v>72.63</v>
+      </c>
       <c r="D111" t="n">
-        <v>61.09096717492692</v>
+        <v>66.15720152074462</v>
       </c>
     </row>
     <row r="112">
@@ -2002,11 +2222,13 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C112" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C112" t="n">
+        <v>72.14</v>
+      </c>
       <c r="D112" t="n">
-        <v>64.24998270941323</v>
+        <v>67.663804239941</v>
       </c>
     </row>
     <row r="113">
@@ -2016,11 +2238,13 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C113" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C113" t="n">
+        <v>72.53</v>
+      </c>
       <c r="D113" t="n">
-        <v>63.1499828584807</v>
+        <v>66.01387849442283</v>
       </c>
     </row>
     <row r="114">
@@ -2030,11 +2254,13 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C114" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C114" t="n">
+        <v>72.84999999999999</v>
+      </c>
       <c r="D114" t="n">
-        <v>63.3489750695681</v>
+        <v>67.57292038790484</v>
       </c>
     </row>
     <row r="115">
@@ -2044,11 +2270,13 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C115" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C115" t="n">
+        <v>73.27</v>
+      </c>
       <c r="D115" t="n">
-        <v>61.37897475389349</v>
+        <v>65.66629754199268</v>
       </c>
     </row>
     <row r="116">
@@ -2058,11 +2286,13 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C116" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C116" t="n">
+        <v>71.34</v>
+      </c>
       <c r="D116" t="n">
-        <v>60.90283697555337</v>
+        <v>66.91875190663168</v>
       </c>
     </row>
     <row r="117">
@@ -2072,11 +2302,13 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C117" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C117" t="n">
+        <v>72.04000000000001</v>
+      </c>
       <c r="D117" t="n">
-        <v>58.98283782339388</v>
+        <v>64.97660929656247</v>
       </c>
     </row>
     <row r="118">
@@ -2086,11 +2318,13 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C118" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C118" t="n">
+        <v>69.88</v>
+      </c>
       <c r="D118" t="n">
-        <v>63.08729491933698</v>
+        <v>66.45787153959689</v>
       </c>
     </row>
     <row r="119">
@@ -2100,11 +2334,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C119" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C119" t="n">
+        <v>69.79000000000001</v>
+      </c>
       <c r="D119" t="n">
-        <v>61.38729532753169</v>
+        <v>65.0098136759735</v>
       </c>
     </row>
     <row r="120">
@@ -2114,11 +2350,13 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C120" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C120" t="n">
+        <v>71.31</v>
+      </c>
       <c r="D120" t="n">
-        <v>62.60755079937822</v>
+        <v>67.25064424706243</v>
       </c>
     </row>
     <row r="121">
@@ -2128,11 +2366,13 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C121" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C121" t="n">
+        <v>71.84</v>
+      </c>
       <c r="D121" t="n">
-        <v>61.25755069718394</v>
+        <v>65.75863674592982</v>
       </c>
     </row>
     <row r="122">
@@ -2142,11 +2382,13 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C122" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C122" t="n">
+        <v>74.59</v>
+      </c>
       <c r="D122" t="n">
-        <v>66.39654264772783</v>
+        <v>70.26364407582626</v>
       </c>
     </row>
     <row r="123">
@@ -2156,11 +2398,13 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C123" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C123" t="n">
+        <v>75.44</v>
+      </c>
       <c r="D123" t="n">
-        <v>65.4565422937744</v>
+        <v>68.95241771970328</v>
       </c>
     </row>
     <row r="124">
@@ -2170,11 +2414,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C124" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C124" t="n">
+        <v>75.41</v>
+      </c>
       <c r="D124" t="n">
-        <v>67.00464835081043</v>
+        <v>70.56467544613383</v>
       </c>
     </row>
     <row r="125">
@@ -2184,11 +2430,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C125" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C125" t="n">
+        <v>76.31999999999999</v>
+      </c>
       <c r="D125" t="n">
-        <v>66.17464868459759</v>
+        <v>69.14094801810307</v>
       </c>
     </row>
     <row r="126">
@@ -2198,11 +2446,13 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C126" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C126" t="n">
+        <v>74.81999999999999</v>
+      </c>
       <c r="D126" t="n">
-        <v>63.96105049419022</v>
+        <v>70.52445168309883</v>
       </c>
     </row>
     <row r="127">
@@ -2212,11 +2462,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C127" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C127" t="n">
+        <v>75.3</v>
+      </c>
       <c r="D127" t="n">
-        <v>63.82105006478719</v>
+        <v>69.469309263621</v>
       </c>
     </row>
     <row r="128">
@@ -2226,11 +2478,13 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C128" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C128" t="n">
+        <v>72.16</v>
+      </c>
       <c r="D128" t="n">
-        <v>65.03742712695617</v>
+        <v>67.64376013621522</v>
       </c>
     </row>
     <row r="129">
@@ -2240,11 +2494,13 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C129" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C129" t="n">
+        <v>72.43000000000001</v>
+      </c>
       <c r="D129" t="n">
-        <v>63.91742640802445</v>
+        <v>66.21469934652318</v>
       </c>
     </row>
     <row r="130">
@@ -2254,11 +2510,13 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C130" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C130" t="n">
+        <v>68.47</v>
+      </c>
       <c r="D130" t="n">
-        <v>60.98135453580653</v>
+        <v>65.97817911172024</v>
       </c>
     </row>
     <row r="131">
@@ -2268,11 +2526,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C131" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C131" t="n">
+        <v>69.39</v>
+      </c>
       <c r="D131" t="n">
-        <v>59.60135473797298</v>
+        <v>64.70230647108058</v>
       </c>
     </row>
     <row r="132">
@@ -2282,11 +2542,13 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C132" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C132" t="n">
+        <v>67.11</v>
+      </c>
       <c r="D132" t="n">
-        <v>62.95230832738024</v>
+        <v>66.39538103856069</v>
       </c>
     </row>
     <row r="133">
@@ -2296,11 +2558,13 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C133" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C133" t="n">
+        <v>66.59</v>
+      </c>
       <c r="D133" t="n">
-        <v>63.52230773031737</v>
+        <v>66.17411995692305</v>
       </c>
     </row>
     <row r="134">
@@ -2310,11 +2574,13 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C134" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C134" t="n">
+        <v>70.56999999999999</v>
+      </c>
       <c r="D134" t="n">
-        <v>66.90752354186495</v>
+        <v>67.49139254927918</v>
       </c>
     </row>
     <row r="135">
@@ -2324,11 +2590,13 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C135" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C135" t="n">
+        <v>70.68000000000001</v>
+      </c>
       <c r="D135" t="n">
-        <v>65.37752384391612</v>
+        <v>66.25987682361738</v>
       </c>
     </row>
     <row r="136">
@@ -2338,11 +2606,13 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C136" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C136" t="n">
+        <v>69.95999999999999</v>
+      </c>
       <c r="D136" t="n">
-        <v>63.79281965484012</v>
+        <v>66.26139396777154</v>
       </c>
     </row>
     <row r="137">
@@ -2352,11 +2622,13 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C137" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C137" t="n">
+        <v>70.77</v>
+      </c>
       <c r="D137" t="n">
-        <v>62.13281778500365</v>
+        <v>64.70066730304099</v>
       </c>
     </row>
     <row r="138">
@@ -2366,11 +2638,13 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C138" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C138" t="n">
+        <v>70.58</v>
+      </c>
       <c r="D138" t="n">
-        <v>64.78169281008977</v>
+        <v>67.0825137639732</v>
       </c>
     </row>
     <row r="139">
@@ -2380,11 +2654,13 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C139" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C139" t="n">
+        <v>71.31999999999999</v>
+      </c>
       <c r="D139" t="n">
-        <v>63.3316925220283</v>
+        <v>65.69522352861044</v>
       </c>
     </row>
     <row r="140">
@@ -2394,11 +2670,13 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C140" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C140" t="n">
+        <v>69.31</v>
+      </c>
       <c r="D140" t="n">
-        <v>62.71364782782761</v>
+        <v>65.67634017431935</v>
       </c>
     </row>
     <row r="141">
@@ -2408,11 +2686,13 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C141" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C141" t="n">
+        <v>69.81999999999999</v>
+      </c>
       <c r="D141" t="n">
-        <v>61.28364791091767</v>
+        <v>64.31934442833203</v>
       </c>
     </row>
     <row r="142">
@@ -2422,11 +2702,13 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C142" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C142" t="n">
+        <v>69.64</v>
+      </c>
       <c r="D142" t="n">
-        <v>63.22387415933423</v>
+        <v>66.42119564973541</v>
       </c>
     </row>
     <row r="143">
@@ -2436,11 +2718,13 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C143" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C143" t="n">
+        <v>70.29000000000001</v>
+      </c>
       <c r="D143" t="n">
-        <v>62.32387370142123</v>
+        <v>65.35634816872782</v>
       </c>
     </row>
     <row r="144">
@@ -2450,11 +2734,13 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C144" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C144" t="n">
+        <v>71.48999999999999</v>
+      </c>
       <c r="D144" t="n">
-        <v>64.73894355811828</v>
+        <v>67.73877438362817</v>
       </c>
     </row>
     <row r="145">
@@ -2464,11 +2750,13 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C145" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C145" t="n">
+        <v>72.2</v>
+      </c>
       <c r="D145" t="n">
-        <v>63.61894388616787</v>
+        <v>66.24501395397928</v>
       </c>
     </row>
     <row r="146">
@@ -2478,11 +2766,13 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C146" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C146" t="n">
+        <v>71.45</v>
+      </c>
       <c r="D146" t="n">
-        <v>64.60367335669012</v>
+        <v>67.23028299215613</v>
       </c>
     </row>
     <row r="147">
@@ -2492,11 +2782,13 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C147" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C147" t="n">
+        <v>71.83</v>
+      </c>
       <c r="D147" t="n">
-        <v>63.30367374434387</v>
+        <v>65.58859049616964</v>
       </c>
     </row>
     <row r="148">
@@ -2506,11 +2798,13 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C148" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C148" t="n">
+        <v>72.33</v>
+      </c>
       <c r="D148" t="n">
-        <v>66.09793104982521</v>
+        <v>68.29335357420977</v>
       </c>
     </row>
     <row r="149">
@@ -2520,11 +2814,13 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C149" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C149" t="n">
+        <v>73.05</v>
+      </c>
       <c r="D149" t="n">
-        <v>64.6679309784856</v>
+        <v>66.76142931062247</v>
       </c>
     </row>
     <row r="150">
@@ -2534,11 +2830,13 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C150" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C150" t="n">
+        <v>69.34999999999999</v>
+      </c>
       <c r="D150" t="n">
-        <v>67.59075595984491</v>
+        <v>68.13829962528536</v>
       </c>
     </row>
     <row r="151">
@@ -2548,11 +2846,13 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C151" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C151" t="n">
+        <v>69.54000000000001</v>
+      </c>
       <c r="D151" t="n">
-        <v>66.22075613251758</v>
+        <v>67.23826594604461</v>
       </c>
     </row>
     <row r="152">
@@ -2562,11 +2862,13 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C152" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C152" t="n">
+        <v>67.75</v>
+      </c>
       <c r="D152" t="n">
-        <v>57.93798455345137</v>
+        <v>65.35448069284054</v>
       </c>
     </row>
     <row r="153">
@@ -2576,11 +2878,13 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C153" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C153" t="n">
+        <v>67.17</v>
+      </c>
       <c r="D153" t="n">
-        <v>56.47798457371542</v>
+        <v>64.27866057559655</v>
       </c>
     </row>
     <row r="154">
@@ -2590,11 +2894,13 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C154" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C154" t="n">
+        <v>72.67</v>
+      </c>
       <c r="D154" t="n">
-        <v>68.64987220847172</v>
+        <v>69.20032807453806</v>
       </c>
     </row>
     <row r="155">
@@ -2604,11 +2910,13 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C155" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C155" t="n">
+        <v>73.55</v>
+      </c>
       <c r="D155" t="n">
-        <v>67.54987252262659</v>
+        <v>68.20729135048578</v>
       </c>
     </row>
     <row r="156">
@@ -2618,11 +2926,13 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C156" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C156" t="n">
+        <v>68.77</v>
+      </c>
       <c r="D156" t="n">
-        <v>62.81123195660784</v>
+        <v>65.98208860654887</v>
       </c>
     </row>
     <row r="157">
@@ -2632,11 +2942,13 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C157" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C157" t="n">
+        <v>70.43000000000001</v>
+      </c>
       <c r="D157" t="n">
-        <v>61.55123224481292</v>
+        <v>64.67944521431205</v>
       </c>
     </row>
     <row r="158">
@@ -2646,11 +2958,13 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C158" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C158" t="n">
+        <v>69.70999999999999</v>
+      </c>
       <c r="D158" t="n">
-        <v>65.06499521849766</v>
+        <v>67.58420750480079</v>
       </c>
     </row>
     <row r="159">
@@ -2660,11 +2974,13 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C159" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C159" t="n">
+        <v>70.06</v>
+      </c>
       <c r="D159" t="n">
-        <v>64.12499488258437</v>
+        <v>66.64050636506582</v>
       </c>
     </row>
     <row r="160">
@@ -2674,11 +2990,13 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C160" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C160" t="n">
+        <v>69.95999999999999</v>
+      </c>
       <c r="D160" t="n">
-        <v>64.70247804888913</v>
+        <v>66.87753076895702</v>
       </c>
     </row>
     <row r="161">
@@ -2688,11 +3006,13 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C161" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C161" t="n">
+        <v>70.33</v>
+      </c>
       <c r="D161" t="n">
-        <v>63.97247894091006</v>
+        <v>65.81060824797486</v>
       </c>
     </row>
     <row r="162">
@@ -2702,11 +3022,13 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C162" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C162" t="n">
+        <v>68.17</v>
+      </c>
       <c r="D162" t="n">
-        <v>62.78496401532129</v>
+        <v>64.90957406919327</v>
       </c>
     </row>
     <row r="163">
@@ -2716,11 +3038,13 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C163" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C163" t="n">
+        <v>68.25</v>
+      </c>
       <c r="D163" t="n">
-        <v>61.72496405416907</v>
+        <v>63.75208476270168</v>
       </c>
     </row>
     <row r="164">
@@ -2730,11 +3054,13 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C164" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C164" t="n">
+        <v>68.45</v>
+      </c>
       <c r="D164" t="n">
-        <v>64.80785567994636</v>
+        <v>66.04197223371571</v>
       </c>
     </row>
     <row r="165">
@@ -2744,11 +3070,13 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C165" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C165" t="n">
+        <v>69.3</v>
+      </c>
       <c r="D165" t="n">
-        <v>63.22785572936579</v>
+        <v>64.93561644795187</v>
       </c>
     </row>
     <row r="166">
@@ -2758,11 +3086,13 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C166" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C166" t="n">
+        <v>70.37</v>
+      </c>
       <c r="D166" t="n">
-        <v>64.77486007303665</v>
+        <v>67.75654125831214</v>
       </c>
     </row>
     <row r="167">
@@ -2772,11 +3102,13 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C167" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C167" t="n">
+        <v>70.22</v>
+      </c>
       <c r="D167" t="n">
-        <v>63.45486038506567</v>
+        <v>66.86721595636686</v>
       </c>
     </row>
     <row r="168">
@@ -2786,11 +3118,13 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C168" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C168" t="n">
+        <v>67.7</v>
+      </c>
       <c r="D168" t="n">
-        <v>61.03454098171649</v>
+        <v>65.7786624031632</v>
       </c>
     </row>
     <row r="169">
@@ -2800,11 +3134,13 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C169" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C169" t="n">
+        <v>68.3</v>
+      </c>
       <c r="D169" t="n">
-        <v>59.62454106659979</v>
+        <v>65.12320118507812</v>
       </c>
     </row>
     <row r="170">
@@ -2814,11 +3150,13 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C170" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="C170" t="n">
+        <v>66.2</v>
+      </c>
       <c r="D170" t="n">
-        <v>66.90790635624876</v>
+        <v>65.75009050653384</v>
       </c>
     </row>
     <row r="171">
@@ -2828,11 +3166,13 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C171" t="inlineStr"/>
+        <v>2023</v>
+      </c>
+      <c r="C171" t="n">
+        <v>66.56</v>
+      </c>
       <c r="D171" t="n">
-        <v>66.33176700842097</v>
+        <v>66.06042091361937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>